<commit_message>
Emit _section psuedo-prompt and show in contents (update template). Show notes in contents by default. Remove obsolete prompt types. Remove pointless afterInitialize.
</commit_message>
<xml_diff>
--- a/form-files/tables/section_test/forms/section_test/section_test.xlsx
+++ b/form-files/tables/section_test/forms/section_test/section_test.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="88">
   <si>
     <t>comments</t>
   </si>
@@ -269,6 +269,24 @@
   </si>
   <si>
     <t>20 साल की उम्र से अधिक होना चाहिए</t>
+  </si>
+  <si>
+    <t>section1</t>
+  </si>
+  <si>
+    <t>section2</t>
+  </si>
+  <si>
+    <t>Section 2</t>
+  </si>
+  <si>
+    <t>Section 1</t>
+  </si>
+  <si>
+    <t>धारा 1</t>
+  </si>
+  <si>
+    <t>धारा 2</t>
   </si>
 </sst>
 </file>
@@ -1176,10 +1194,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1250,29 +1268,57 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>16</v>
+        <v>82</v>
       </c>
       <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" t="s">
-        <v>32</v>
-      </c>
+      <c r="C5" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4" t="s">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F8" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>